<commit_message>
add tsne plot to script v0.21
Note: only the chosen words are plotted using t-sne.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -28,406 +28,406 @@
     <t>革命</t>
   </si>
   <si>
+    <t>胜利</t>
+  </si>
+  <si>
+    <t>实行</t>
+  </si>
+  <si>
+    <t>过程</t>
+  </si>
+  <si>
+    <t>民族</t>
+  </si>
+  <si>
+    <t>改造</t>
+  </si>
+  <si>
+    <t>解放</t>
+  </si>
+  <si>
+    <t>精神</t>
+  </si>
+  <si>
+    <t>美国</t>
+  </si>
+  <si>
+    <t>利益</t>
+  </si>
+  <si>
+    <t>执行</t>
+  </si>
+  <si>
+    <t>青年</t>
+  </si>
+  <si>
+    <t>历史</t>
+  </si>
+  <si>
+    <t>资本主义</t>
+  </si>
+  <si>
+    <t>发展</t>
+  </si>
+  <si>
+    <t>国家</t>
+  </si>
+  <si>
+    <t>反动派</t>
+  </si>
+  <si>
+    <t>全世界</t>
+  </si>
+  <si>
+    <t>机关</t>
+  </si>
+  <si>
+    <t>服从</t>
+  </si>
+  <si>
+    <t>破坏</t>
+  </si>
+  <si>
+    <t>武器</t>
+  </si>
+  <si>
+    <t>教育</t>
+  </si>
+  <si>
+    <t>无产阶级</t>
+  </si>
+  <si>
+    <t>错误</t>
+  </si>
+  <si>
+    <t>之间</t>
+  </si>
+  <si>
+    <t>情况</t>
+  </si>
+  <si>
+    <t>一种</t>
+  </si>
+  <si>
+    <t>斗争</t>
+  </si>
+  <si>
+    <t>目的</t>
+  </si>
+  <si>
+    <t>团结</t>
+  </si>
+  <si>
+    <t>内部</t>
+  </si>
+  <si>
+    <t>反革命</t>
+  </si>
+  <si>
+    <t>事物</t>
+  </si>
+  <si>
+    <t>懂得</t>
+  </si>
+  <si>
+    <t>地位</t>
+  </si>
+  <si>
+    <t>地方</t>
+  </si>
+  <si>
+    <t>自由</t>
+  </si>
+  <si>
+    <t>客观</t>
+  </si>
+  <si>
+    <t>调查</t>
+  </si>
+  <si>
+    <t>作风</t>
+  </si>
+  <si>
+    <t>实践</t>
+  </si>
+  <si>
+    <t>阶级</t>
+  </si>
+  <si>
+    <t>组织</t>
+  </si>
+  <si>
+    <t>消灭</t>
+  </si>
+  <si>
+    <t>解决</t>
+  </si>
+  <si>
+    <t>我国</t>
+  </si>
+  <si>
+    <t>建立</t>
+  </si>
+  <si>
+    <t>制度</t>
+  </si>
+  <si>
+    <t>社会</t>
+  </si>
+  <si>
+    <t>条件</t>
+  </si>
+  <si>
+    <t>阶段</t>
+  </si>
+  <si>
+    <t>表现</t>
+  </si>
+  <si>
+    <t>和平</t>
+  </si>
+  <si>
+    <t>工作</t>
+  </si>
+  <si>
+    <t>发生</t>
+  </si>
+  <si>
+    <t>批评</t>
+  </si>
+  <si>
+    <t>原则</t>
+  </si>
+  <si>
+    <t>共产党员</t>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <t>时期</t>
+  </si>
+  <si>
+    <t>艺术</t>
+  </si>
+  <si>
+    <t>中国共产党</t>
+  </si>
+  <si>
+    <t>正确</t>
+  </si>
+  <si>
+    <t>农业</t>
+  </si>
+  <si>
+    <t>性质</t>
+  </si>
+  <si>
+    <t>群众</t>
+  </si>
+  <si>
+    <t>关系</t>
+  </si>
+  <si>
+    <t>知识分子</t>
+  </si>
+  <si>
+    <t>马克思列宁主义</t>
+  </si>
+  <si>
+    <t>马克思主义</t>
+  </si>
+  <si>
+    <t>阶级斗争</t>
+  </si>
+  <si>
+    <t>反对</t>
+  </si>
+  <si>
+    <t>两个</t>
+  </si>
+  <si>
+    <t>善于</t>
+  </si>
+  <si>
+    <t>劳动</t>
+  </si>
+  <si>
+    <t>成绩</t>
+  </si>
+  <si>
+    <t>研究</t>
+  </si>
+  <si>
+    <t>积极性</t>
+  </si>
+  <si>
+    <t>一部分</t>
+  </si>
+  <si>
+    <t>理论</t>
+  </si>
+  <si>
+    <t>事情</t>
+  </si>
+  <si>
+    <t>政策</t>
+  </si>
+  <si>
+    <t>农民</t>
+  </si>
+  <si>
+    <t>敌人</t>
+  </si>
+  <si>
+    <t>办法</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>分析</t>
+  </si>
+  <si>
+    <t>态度</t>
+  </si>
+  <si>
+    <t>只能</t>
+  </si>
+  <si>
+    <t>军事</t>
+  </si>
+  <si>
+    <t>缺点</t>
+  </si>
+  <si>
+    <t>党内</t>
+  </si>
+  <si>
+    <t>纪律</t>
+  </si>
+  <si>
+    <t>东西</t>
+  </si>
+  <si>
+    <t>资产阶级</t>
+  </si>
+  <si>
+    <t>修正主义</t>
+  </si>
+  <si>
+    <t>方法</t>
+  </si>
+  <si>
+    <t>战争</t>
+  </si>
+  <si>
+    <t>共产党</t>
+  </si>
+  <si>
+    <t>士兵</t>
+  </si>
+  <si>
+    <t>干部</t>
+  </si>
+  <si>
+    <t>事业</t>
+  </si>
+  <si>
+    <t>力量</t>
+  </si>
+  <si>
+    <t>基础</t>
+  </si>
+  <si>
     <t>军队</t>
   </si>
   <si>
-    <t>作风</t>
+    <t>领导</t>
+  </si>
+  <si>
+    <t>经验</t>
+  </si>
+  <si>
+    <t>党员</t>
+  </si>
+  <si>
+    <t>观点</t>
+  </si>
+  <si>
+    <t>矛盾</t>
+  </si>
+  <si>
+    <t>世界</t>
+  </si>
+  <si>
+    <t>思想</t>
+  </si>
+  <si>
+    <t>共产党人</t>
+  </si>
+  <si>
+    <t>一点</t>
+  </si>
+  <si>
+    <t>工人阶级</t>
+  </si>
+  <si>
+    <t>建设</t>
+  </si>
+  <si>
+    <t>意见</t>
+  </si>
+  <si>
+    <t>参加</t>
+  </si>
+  <si>
+    <t>民主</t>
+  </si>
+  <si>
+    <t>民众</t>
+  </si>
+  <si>
+    <t>打仗</t>
+  </si>
+  <si>
+    <t>出发</t>
+  </si>
+  <si>
+    <t>同志</t>
+  </si>
+  <si>
+    <t>经济</t>
+  </si>
+  <si>
+    <t>学习</t>
+  </si>
+  <si>
+    <t>失败</t>
+  </si>
+  <si>
+    <t>生产</t>
+  </si>
+  <si>
+    <t>困难</t>
+  </si>
+  <si>
+    <t>服务</t>
+  </si>
+  <si>
+    <t>计划</t>
   </si>
   <si>
     <t>运动</t>
   </si>
   <si>
-    <t>教育</t>
-  </si>
-  <si>
-    <t>过程</t>
-  </si>
-  <si>
-    <t>农民</t>
-  </si>
-  <si>
-    <t>修正主义</t>
-  </si>
-  <si>
-    <t>一种</t>
-  </si>
-  <si>
-    <t>团结</t>
-  </si>
-  <si>
-    <t>一点</t>
-  </si>
-  <si>
-    <t>工人阶级</t>
-  </si>
-  <si>
-    <t>战争</t>
-  </si>
-  <si>
-    <t>地位</t>
-  </si>
-  <si>
-    <t>执行</t>
-  </si>
-  <si>
-    <t>打仗</t>
-  </si>
-  <si>
-    <t>地方</t>
-  </si>
-  <si>
-    <t>日本</t>
-  </si>
-  <si>
-    <t>失败</t>
-  </si>
-  <si>
-    <t>困难</t>
-  </si>
-  <si>
-    <t>调查</t>
-  </si>
-  <si>
-    <t>破坏</t>
-  </si>
-  <si>
-    <t>党内</t>
-  </si>
-  <si>
-    <t>青年</t>
-  </si>
-  <si>
-    <t>纪律</t>
-  </si>
-  <si>
-    <t>错误</t>
-  </si>
-  <si>
-    <t>我国</t>
-  </si>
-  <si>
-    <t>阶段</t>
-  </si>
-  <si>
-    <t>反革命</t>
-  </si>
-  <si>
-    <t>表现</t>
-  </si>
-  <si>
-    <t>分析</t>
-  </si>
-  <si>
-    <t>美国</t>
-  </si>
-  <si>
-    <t>群众</t>
-  </si>
-  <si>
-    <t>发生</t>
-  </si>
-  <si>
-    <t>武器</t>
-  </si>
-  <si>
-    <t>政策</t>
-  </si>
-  <si>
-    <t>经验</t>
-  </si>
-  <si>
-    <t>历史</t>
-  </si>
-  <si>
-    <t>东西</t>
-  </si>
-  <si>
-    <t>国家</t>
-  </si>
-  <si>
-    <t>工作</t>
-  </si>
-  <si>
-    <t>出发</t>
-  </si>
-  <si>
-    <t>服务</t>
-  </si>
-  <si>
-    <t>中国共产党</t>
-  </si>
-  <si>
-    <t>力量</t>
-  </si>
-  <si>
-    <t>基础</t>
-  </si>
-  <si>
-    <t>马克思列宁主义</t>
-  </si>
-  <si>
-    <t>胜利</t>
-  </si>
-  <si>
-    <t>事情</t>
-  </si>
-  <si>
-    <t>正确</t>
-  </si>
-  <si>
-    <t>实践</t>
-  </si>
-  <si>
-    <t>消灭</t>
-  </si>
-  <si>
-    <t>敌人</t>
-  </si>
-  <si>
-    <t>之间</t>
-  </si>
-  <si>
-    <t>资本主义</t>
-  </si>
-  <si>
-    <t>解决</t>
-  </si>
-  <si>
-    <t>思想</t>
-  </si>
-  <si>
-    <t>共产党人</t>
-  </si>
-  <si>
-    <t>参加</t>
-  </si>
-  <si>
-    <t>事物</t>
-  </si>
-  <si>
-    <t>共产党</t>
-  </si>
-  <si>
-    <t>态度</t>
-  </si>
-  <si>
-    <t>民众</t>
-  </si>
-  <si>
-    <t>原则</t>
-  </si>
-  <si>
-    <t>积极性</t>
-  </si>
-  <si>
-    <t>时期</t>
-  </si>
-  <si>
-    <t>生产</t>
-  </si>
-  <si>
-    <t>计划</t>
-  </si>
-  <si>
-    <t>艺术</t>
-  </si>
-  <si>
-    <t>理论</t>
-  </si>
-  <si>
-    <t>实行</t>
-  </si>
-  <si>
-    <t>阶级</t>
-  </si>
-  <si>
-    <t>阶级斗争</t>
-  </si>
-  <si>
-    <t>观点</t>
-  </si>
-  <si>
-    <t>矛盾</t>
-  </si>
-  <si>
-    <t>民族</t>
-  </si>
-  <si>
-    <t>时间</t>
-  </si>
-  <si>
-    <t>建立</t>
-  </si>
-  <si>
-    <t>情况</t>
-  </si>
-  <si>
-    <t>发展</t>
-  </si>
-  <si>
-    <t>善于</t>
-  </si>
-  <si>
-    <t>机关</t>
-  </si>
-  <si>
-    <t>士兵</t>
-  </si>
-  <si>
-    <t>自由</t>
-  </si>
-  <si>
-    <t>客观</t>
-  </si>
-  <si>
-    <t>服从</t>
-  </si>
-  <si>
-    <t>马克思主义</t>
-  </si>
-  <si>
-    <t>改造</t>
-  </si>
-  <si>
-    <t>世界</t>
-  </si>
-  <si>
-    <t>解放</t>
-  </si>
-  <si>
-    <t>目的</t>
-  </si>
-  <si>
-    <t>反动派</t>
-  </si>
-  <si>
-    <t>只能</t>
-  </si>
-  <si>
-    <t>军事</t>
-  </si>
-  <si>
-    <t>批评</t>
+    <t>标准</t>
+  </si>
+  <si>
+    <t>政治</t>
   </si>
   <si>
     <t>生活</t>
-  </si>
-  <si>
-    <t>经济</t>
-  </si>
-  <si>
-    <t>知识分子</t>
-  </si>
-  <si>
-    <t>资产阶级</t>
-  </si>
-  <si>
-    <t>制度</t>
-  </si>
-  <si>
-    <t>内部</t>
-  </si>
-  <si>
-    <t>和平</t>
-  </si>
-  <si>
-    <t>劳动</t>
-  </si>
-  <si>
-    <t>一部分</t>
-  </si>
-  <si>
-    <t>干部</t>
-  </si>
-  <si>
-    <t>事业</t>
-  </si>
-  <si>
-    <t>性质</t>
-  </si>
-  <si>
-    <t>政治</t>
-  </si>
-  <si>
-    <t>关系</t>
-  </si>
-  <si>
-    <t>成绩</t>
-  </si>
-  <si>
-    <t>领导</t>
-  </si>
-  <si>
-    <t>党员</t>
-  </si>
-  <si>
-    <t>组织</t>
-  </si>
-  <si>
-    <t>办法</t>
-  </si>
-  <si>
-    <t>反对</t>
-  </si>
-  <si>
-    <t>无产阶级</t>
-  </si>
-  <si>
-    <t>斗争</t>
-  </si>
-  <si>
-    <t>社会</t>
-  </si>
-  <si>
-    <t>农业</t>
-  </si>
-  <si>
-    <t>条件</t>
-  </si>
-  <si>
-    <t>方法</t>
-  </si>
-  <si>
-    <t>建设</t>
-  </si>
-  <si>
-    <t>标准</t>
-  </si>
-  <si>
-    <t>意见</t>
-  </si>
-  <si>
-    <t>民主</t>
-  </si>
-  <si>
-    <t>精神</t>
-  </si>
-  <si>
-    <t>全世界</t>
-  </si>
-  <si>
-    <t>利益</t>
-  </si>
-  <si>
-    <t>研究</t>
-  </si>
-  <si>
-    <t>同志</t>
-  </si>
-  <si>
-    <t>共产党员</t>
-  </si>
-  <si>
-    <t>缺点</t>
-  </si>
-  <si>
-    <t>两个</t>
-  </si>
-  <si>
-    <t>懂得</t>
-  </si>
-  <si>
-    <t>学习</t>
   </si>
 </sst>
 </file>
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.004818503051718599</v>
+        <v>0.00329264375200771</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -841,7 +841,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>0.00104400899453903</v>
+        <v>0.00305171859942178</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -855,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>0.002489559910054609</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -869,7 +869,7 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>0.00136524253132027</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -883,7 +883,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>0.00128493414712496</v>
+        <v>0.0024092515258593</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -897,7 +897,7 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>0.00208801798907806</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -911,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>0.00112431737873434</v>
+        <v>0.00208801798907806</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -925,7 +925,7 @@
         <v>11</v>
       </c>
       <c r="D10">
-        <v>0.00224863475746868</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -939,7 +939,7 @@
         <v>12</v>
       </c>
       <c r="D11">
-        <v>0.004336652746546739</v>
+        <v>0.00265017667844523</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -953,7 +953,7 @@
         <v>13</v>
       </c>
       <c r="D12">
-        <v>0.00168647606810151</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -967,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>0.0016061676839062</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -975,13 +975,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
       <c r="D14">
-        <v>0.005862512046257629</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -989,13 +989,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15">
-        <v>0.00128493414712496</v>
+        <v>0.00168647606810151</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1003,13 +1003,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16">
-        <v>0.00120462576292965</v>
+        <v>0.003854802441374879</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1017,13 +1017,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17">
-        <v>0.00104400899453903</v>
+        <v>0.00409572759396081</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1031,13 +1031,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18">
-        <v>0.00168647606810151</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1045,13 +1045,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
       </c>
       <c r="D19">
-        <v>0.00104400899453903</v>
+        <v>0.00136524253132027</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1059,7 +1059,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -1073,13 +1073,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
       <c r="D21">
-        <v>0.00208801798907806</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1087,13 +1087,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
       </c>
       <c r="D22">
-        <v>0.00144555091551558</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1101,13 +1101,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
         <v>24</v>
       </c>
       <c r="D23">
-        <v>0.00104400899453903</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1115,7 +1115,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
@@ -1129,13 +1129,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
       </c>
       <c r="D25">
-        <v>0.00128493414712496</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1143,13 +1143,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26">
-        <v>0.00144555091551558</v>
+        <v>0.00457757789913267</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1157,13 +1157,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
       </c>
       <c r="D27">
-        <v>0.00457757789913267</v>
+        <v>0.00305171859942178</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1171,13 +1171,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
       <c r="D28">
-        <v>0.00200770960488275</v>
+        <v>0.00305171859942178</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1185,13 +1185,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
       </c>
       <c r="D29">
-        <v>0.00104400899453903</v>
+        <v>0.00224863475746868</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1199,13 +1199,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
         <v>31</v>
       </c>
       <c r="D30">
-        <v>0.00112431737873434</v>
+        <v>0.00530035335689046</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1213,13 +1213,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
       </c>
       <c r="D31">
-        <v>0.00112431737873434</v>
+        <v>0.00144555091551558</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1227,13 +1227,13 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
       </c>
       <c r="D32">
-        <v>0.0016061676839062</v>
+        <v>0.004336652746546739</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1241,13 +1241,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
       </c>
       <c r="D33">
-        <v>0.00104400899453903</v>
+        <v>0.00305171859942178</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1255,13 +1255,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
         <v>35</v>
       </c>
       <c r="D34">
-        <v>0.01068101509797623</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1269,13 +1269,13 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
       </c>
       <c r="D35">
-        <v>0.00112431737873434</v>
+        <v>0.00289110183103116</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1289,7 +1289,7 @@
         <v>37</v>
       </c>
       <c r="D36">
-        <v>0.00120462576292965</v>
+        <v>0.00176678445229682</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1303,7 +1303,7 @@
         <v>38</v>
       </c>
       <c r="D37">
-        <v>0.00273048506264054</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1317,7 +1317,7 @@
         <v>39</v>
       </c>
       <c r="D38">
-        <v>0.00152585929971089</v>
+        <v>0.00168647606810151</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1331,7 +1331,7 @@
         <v>40</v>
       </c>
       <c r="D39">
-        <v>0.00232894314166399</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1345,7 +1345,7 @@
         <v>41</v>
       </c>
       <c r="D40">
-        <v>0.00192740122068744</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1359,7 +1359,7 @@
         <v>42</v>
       </c>
       <c r="D41">
-        <v>0.00409572759396081</v>
+        <v>0.00144555091551558</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1367,13 +1367,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
         <v>43</v>
       </c>
       <c r="D42">
-        <v>0.01092194025056216</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1381,13 +1381,13 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
       </c>
       <c r="D43">
-        <v>0.00120462576292965</v>
+        <v>0.00192740122068744</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1395,13 +1395,13 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
       </c>
       <c r="D44">
-        <v>0.00104400899453903</v>
+        <v>0.00337295213620302</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1415,7 +1415,7 @@
         <v>46</v>
       </c>
       <c r="D45">
-        <v>0.00104400899453903</v>
+        <v>0.00256986829424992</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1429,7 +1429,7 @@
         <v>47</v>
       </c>
       <c r="D46">
-        <v>0.00224863475746868</v>
+        <v>0.00337295213620302</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1443,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="D47">
-        <v>0.00136524253132027</v>
+        <v>0.00393511082557019</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1457,7 +1457,7 @@
         <v>49</v>
       </c>
       <c r="D48">
-        <v>0.0016061676839062</v>
+        <v>0.00200770960488275</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1471,7 +1471,7 @@
         <v>50</v>
       </c>
       <c r="D49">
-        <v>0.00329264375200771</v>
+        <v>0.0016061676839062</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1485,7 +1485,7 @@
         <v>51</v>
       </c>
       <c r="D50">
-        <v>0.00176678445229682</v>
+        <v>0.00208801798907806</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1499,7 +1499,7 @@
         <v>52</v>
       </c>
       <c r="D51">
-        <v>0.004176035978156119</v>
+        <v>0.00409572759396081</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1513,7 +1513,7 @@
         <v>53</v>
       </c>
       <c r="D52">
-        <v>0.00192740122068744</v>
+        <v>0.00152585929971089</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1527,7 +1527,7 @@
         <v>54</v>
       </c>
       <c r="D53">
-        <v>0.00337295213620302</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1541,7 +1541,7 @@
         <v>55</v>
       </c>
       <c r="D54">
-        <v>0.006424670735624799</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1555,7 +1555,7 @@
         <v>56</v>
       </c>
       <c r="D55">
-        <v>0.00305171859942178</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1569,7 +1569,7 @@
         <v>57</v>
       </c>
       <c r="D56">
-        <v>0.00168647606810151</v>
+        <v>0.01092194025056216</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1583,7 +1583,7 @@
         <v>58</v>
       </c>
       <c r="D57">
-        <v>0.00393511082557019</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1597,7 +1597,7 @@
         <v>59</v>
       </c>
       <c r="D58">
-        <v>0.004497269514937359</v>
+        <v>0.00305171859942178</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1611,7 +1611,7 @@
         <v>60</v>
       </c>
       <c r="D59">
-        <v>0.00112431737873434</v>
+        <v>0.00273048506264054</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1625,7 +1625,7 @@
         <v>61</v>
       </c>
       <c r="D60">
-        <v>0.00136524253132027</v>
+        <v>0.00256986829424992</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1639,7 +1639,7 @@
         <v>62</v>
       </c>
       <c r="D61">
-        <v>0.00289110183103116</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1667,7 +1667,7 @@
         <v>64</v>
       </c>
       <c r="D63">
-        <v>0.00232894314166399</v>
+        <v>0.00176678445229682</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1675,7 +1675,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C64" t="s">
         <v>65</v>
@@ -1689,13 +1689,13 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
         <v>66</v>
       </c>
       <c r="D65">
-        <v>0.00273048506264054</v>
+        <v>0.004176035978156119</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1703,13 +1703,13 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
         <v>67</v>
       </c>
       <c r="D66">
-        <v>0.00144555091551558</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1717,13 +1717,13 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C67" t="s">
         <v>68</v>
       </c>
       <c r="D67">
-        <v>0.0016061676839062</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1731,13 +1731,13 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
         <v>69</v>
       </c>
       <c r="D68">
-        <v>0.00297141021522647</v>
+        <v>0.01068101509797623</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1745,13 +1745,13 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C69" t="s">
         <v>70</v>
       </c>
       <c r="D69">
-        <v>0.00104400899453903</v>
+        <v>0.00152585929971089</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1759,13 +1759,13 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
         <v>71</v>
       </c>
       <c r="D70">
-        <v>0.00176678445229682</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1773,13 +1773,13 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
         <v>72</v>
       </c>
       <c r="D71">
-        <v>0.00224863475746868</v>
+        <v>0.0016061676839062</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1787,13 +1787,13 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
         <v>73</v>
       </c>
       <c r="D72">
-        <v>0.00305171859942178</v>
+        <v>0.00289110183103116</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1801,13 +1801,13 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
         <v>74</v>
       </c>
       <c r="D73">
-        <v>0.00337295213620302</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1815,13 +1815,13 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
         <v>75</v>
       </c>
       <c r="D74">
-        <v>0.00128493414712496</v>
+        <v>0.0032123353678124</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1829,7 +1829,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
         <v>76</v>
@@ -1843,13 +1843,13 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
         <v>77</v>
       </c>
       <c r="D76">
-        <v>0.006585287504015419</v>
+        <v>0.00184709283649213</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1857,13 +1857,13 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
         <v>78</v>
       </c>
       <c r="D77">
-        <v>0.00232894314166399</v>
+        <v>0.00208801798907806</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1871,13 +1871,13 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
         <v>79</v>
       </c>
       <c r="D78">
-        <v>0.00120462576292965</v>
+        <v>0.00152585929971089</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1885,13 +1885,13 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
         <v>80</v>
       </c>
       <c r="D79">
-        <v>0.0016061676839062</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1899,13 +1899,13 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
         <v>81</v>
       </c>
       <c r="D80">
-        <v>0.00305171859942178</v>
+        <v>0.00144555091551558</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1913,13 +1913,13 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
         <v>82</v>
       </c>
       <c r="D81">
-        <v>0.003854802441374879</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1927,13 +1927,13 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
         <v>83</v>
       </c>
       <c r="D82">
-        <v>0.00184709283649213</v>
+        <v>0.00224863475746868</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1941,13 +1941,13 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
         <v>84</v>
       </c>
       <c r="D83">
-        <v>0.00152585929971089</v>
+        <v>0.00176678445229682</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1955,13 +1955,13 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
         <v>85</v>
       </c>
       <c r="D84">
-        <v>0.00128493414712496</v>
+        <v>0.00273048506264054</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1969,13 +1969,13 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
         <v>86</v>
       </c>
       <c r="D85">
-        <v>0.00120462576292965</v>
+        <v>0.00208801798907806</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1983,13 +1983,13 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
         <v>87</v>
       </c>
       <c r="D86">
-        <v>0.00120462576292965</v>
+        <v>0.006424670735624799</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1997,13 +1997,13 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
         <v>88</v>
       </c>
       <c r="D87">
-        <v>0.00120462576292965</v>
+        <v>0.00168647606810151</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2011,13 +2011,13 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C88" t="s">
         <v>89</v>
       </c>
       <c r="D88">
-        <v>0.00289110183103116</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2025,13 +2025,13 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C89" t="s">
         <v>90</v>
       </c>
       <c r="D89">
-        <v>0.0024092515258593</v>
+        <v>0.0016061676839062</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2039,13 +2039,13 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C90" t="s">
         <v>91</v>
       </c>
       <c r="D90">
-        <v>0.00265017667844523</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2053,13 +2053,13 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s">
         <v>92</v>
       </c>
       <c r="D91">
-        <v>0.00120462576292965</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2067,13 +2067,13 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C92" t="s">
         <v>93</v>
       </c>
       <c r="D92">
-        <v>0.00144555091551558</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2081,13 +2081,13 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
         <v>94</v>
       </c>
       <c r="D93">
-        <v>0.00232894314166399</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2095,13 +2095,13 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
         <v>95</v>
       </c>
       <c r="D94">
-        <v>0.00104400899453903</v>
+        <v>0.00136524253132027</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2109,13 +2109,13 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C95" t="s">
         <v>96</v>
       </c>
       <c r="D95">
-        <v>0.00104400899453903</v>
+        <v>0.00144555091551558</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2123,13 +2123,13 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C96" t="s">
         <v>97</v>
       </c>
       <c r="D96">
-        <v>0.00305171859942178</v>
+        <v>0.00192740122068744</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2137,13 +2137,13 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C97" t="s">
         <v>98</v>
       </c>
       <c r="D97">
-        <v>0.00232894314166399</v>
+        <v>0.00329264375200771</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2151,13 +2151,13 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C98" t="s">
         <v>99</v>
       </c>
       <c r="D98">
-        <v>0.00128493414712496</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2165,13 +2165,13 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C99" t="s">
         <v>100</v>
       </c>
       <c r="D99">
-        <v>0.00120462576292965</v>
+        <v>0.0056215868936717</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2179,13 +2179,13 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C100" t="s">
         <v>101</v>
       </c>
       <c r="D100">
-        <v>0.00329264375200771</v>
+        <v>0.005862512046257629</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2193,13 +2193,13 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C101" t="s">
         <v>102</v>
       </c>
       <c r="D101">
-        <v>0.00208801798907806</v>
+        <v>0.0016061676839062</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2207,13 +2207,13 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C102" t="s">
         <v>103</v>
       </c>
       <c r="D102">
-        <v>0.00305171859942178</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2221,13 +2221,13 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C103" t="s">
         <v>104</v>
       </c>
       <c r="D103">
-        <v>0.00112431737873434</v>
+        <v>0.003774494057179569</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2235,13 +2235,13 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C104" t="s">
         <v>105</v>
       </c>
       <c r="D104">
-        <v>0.00208801798907806</v>
+        <v>0.00216832637327337</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2249,13 +2249,13 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C105" t="s">
         <v>106</v>
       </c>
       <c r="D105">
-        <v>0.00104400899453903</v>
+        <v>0.00224863475746868</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2263,13 +2263,13 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C106" t="s">
         <v>107</v>
       </c>
       <c r="D106">
-        <v>0.003774494057179569</v>
+        <v>0.00136524253132027</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2277,13 +2277,13 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C107" t="s">
         <v>108</v>
       </c>
       <c r="D107">
-        <v>0.00216832637327337</v>
+        <v>0.004818503051718599</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2291,13 +2291,13 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C108" t="s">
         <v>109</v>
       </c>
       <c r="D108">
-        <v>0.00112431737873434</v>
+        <v>0.005059428204304529</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2305,13 +2305,13 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C109" t="s">
         <v>110</v>
       </c>
       <c r="D109">
-        <v>0.006585287504015419</v>
+        <v>0.00152585929971089</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2319,13 +2319,13 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C110" t="s">
         <v>111</v>
       </c>
       <c r="D110">
-        <v>0.00152585929971089</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2333,13 +2333,13 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C111" t="s">
         <v>112</v>
       </c>
       <c r="D111">
-        <v>0.00152585929971089</v>
+        <v>0.00144555091551558</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2353,7 +2353,7 @@
         <v>113</v>
       </c>
       <c r="D112">
-        <v>0.005059428204304529</v>
+        <v>0.006585287504015419</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2367,7 +2367,7 @@
         <v>114</v>
       </c>
       <c r="D113">
-        <v>0.00112431737873434</v>
+        <v>0.00265017667844523</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2381,7 +2381,7 @@
         <v>115</v>
       </c>
       <c r="D114">
-        <v>0.00256986829424992</v>
+        <v>0.004497269514937359</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2395,7 +2395,7 @@
         <v>116</v>
       </c>
       <c r="D115">
-        <v>0.00168647606810151</v>
+        <v>0.00112431737873434</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2409,7 +2409,7 @@
         <v>117</v>
       </c>
       <c r="D116">
-        <v>0.0032123353678124</v>
+        <v>0.00168647606810151</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2423,7 +2423,7 @@
         <v>118</v>
       </c>
       <c r="D117">
-        <v>0.00232894314166399</v>
+        <v>0.0016061676839062</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2437,7 +2437,7 @@
         <v>119</v>
       </c>
       <c r="D118">
-        <v>0.00530035335689046</v>
+        <v>0.00184709283649213</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2451,7 +2451,7 @@
         <v>120</v>
       </c>
       <c r="D119">
-        <v>0.00409572759396081</v>
+        <v>0.00208801798907806</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2465,7 +2465,7 @@
         <v>121</v>
       </c>
       <c r="D120">
-        <v>0.00128493414712496</v>
+        <v>0.00136524253132027</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2479,7 +2479,7 @@
         <v>122</v>
       </c>
       <c r="D121">
-        <v>0.00152585929971089</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2493,7 +2493,7 @@
         <v>123</v>
       </c>
       <c r="D122">
-        <v>0.0056215868936717</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2507,7 +2507,7 @@
         <v>124</v>
       </c>
       <c r="D123">
-        <v>0.00184709283649213</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2521,7 +2521,7 @@
         <v>125</v>
       </c>
       <c r="D124">
-        <v>0.00136524253132027</v>
+        <v>0.00120462576292965</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2535,7 +2535,7 @@
         <v>126</v>
       </c>
       <c r="D125">
-        <v>0.00208801798907806</v>
+        <v>0.004015419209765499</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2549,7 +2549,7 @@
         <v>127</v>
       </c>
       <c r="D126">
-        <v>0.00232894314166399</v>
+        <v>0.00128493414712496</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2563,7 +2563,7 @@
         <v>128</v>
       </c>
       <c r="D127">
-        <v>0.00208801798907806</v>
+        <v>0.00281079344683585</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2577,7 +2577,7 @@
         <v>129</v>
       </c>
       <c r="D128">
-        <v>0.00136524253132027</v>
+        <v>0.00152585929971089</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2591,7 +2591,7 @@
         <v>130</v>
       </c>
       <c r="D129">
-        <v>0.00265017667844523</v>
+        <v>0.00297141021522647</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2605,7 +2605,7 @@
         <v>131</v>
       </c>
       <c r="D130">
-        <v>0.00120462576292965</v>
+        <v>0.00208801798907806</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2619,7 +2619,7 @@
         <v>132</v>
       </c>
       <c r="D131">
-        <v>0.004015419209765499</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2633,7 +2633,7 @@
         <v>133</v>
       </c>
       <c r="D132">
-        <v>0.00256986829424992</v>
+        <v>0.00104400899453903</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2641,13 +2641,13 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C133" t="s">
         <v>134</v>
       </c>
       <c r="D133">
-        <v>0.00128493414712496</v>
+        <v>0.002489559910054609</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2661,7 +2661,7 @@
         <v>135</v>
       </c>
       <c r="D134">
-        <v>0.00144555091551558</v>
+        <v>0.00136524253132027</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2675,7 +2675,7 @@
         <v>136</v>
       </c>
       <c r="D135">
-        <v>0.00176678445229682</v>
+        <v>0.006585287504015419</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2689,7 +2689,7 @@
         <v>137</v>
       </c>
       <c r="D136">
-        <v>0.00281079344683585</v>
+        <v>0.00232894314166399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>